<commit_message>
Cliente especial sempre no caminhão 1 pronto, Sofás por tamanho do caminhão iniciado
</commit_message>
<xml_diff>
--- a/Data/nova_planilha_local.xlsx
+++ b/Data/nova_planilha_local.xlsx
@@ -577,7 +577,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -785,7 +785,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -989,7 +989,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -2993,7 +2993,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -4659,7 +4659,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -4757,7 +4757,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -5443,7 +5443,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -6423,7 +6423,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -6619,7 +6619,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -6913,7 +6913,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -7011,7 +7011,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -7207,7 +7207,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -7305,7 +7305,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -7501,7 +7501,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -7599,7 +7599,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -7795,7 +7795,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -7991,7 +7991,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -8579,7 +8579,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -8873,7 +8873,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -9167,7 +9167,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -9265,7 +9265,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -9853,7 +9853,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -9951,7 +9951,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -10049,7 +10049,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -10343,7 +10343,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -10537,7 +10537,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -10913,7 +10913,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -11101,7 +11101,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
@@ -11195,7 +11195,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -11289,7 +11289,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -11383,7 +11383,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -11477,7 +11477,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -11571,7 +11571,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -11665,7 +11665,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -11759,7 +11759,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -11947,7 +11947,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -12041,7 +12041,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -12135,7 +12135,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -12417,7 +12417,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -12605,7 +12605,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -12699,7 +12699,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -12793,7 +12793,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -12981,7 +12981,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -13169,7 +13169,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -13263,7 +13263,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -13357,7 +13357,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -13545,7 +13545,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
@@ -13639,7 +13639,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
@@ -13733,7 +13733,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -14109,7 +14109,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -14203,7 +14203,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -14485,7 +14485,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -14767,7 +14767,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -14861,7 +14861,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -14955,7 +14955,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -15049,7 +15049,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -15237,7 +15237,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -15331,7 +15331,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
@@ -15425,7 +15425,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -15613,7 +15613,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -15895,7 +15895,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -15989,7 +15989,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -16177,7 +16177,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C163" t="inlineStr"/>
@@ -16271,7 +16271,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -16459,7 +16459,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C166" t="inlineStr"/>
@@ -16647,7 +16647,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -16929,7 +16929,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
@@ -17023,7 +17023,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>
@@ -17211,7 +17211,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>20/11/2024</t>
         </is>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -17399,7 +17399,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -17681,7 +17681,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -17869,7 +17869,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
@@ -17963,7 +17963,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -18151,7 +18151,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -18245,7 +18245,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -18339,7 +18339,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -18433,7 +18433,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -18621,7 +18621,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C189" t="inlineStr"/>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C190" t="inlineStr"/>
@@ -18903,7 +18903,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>21/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -19091,7 +19091,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -19185,7 +19185,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -19279,7 +19279,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -19373,7 +19373,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -19467,7 +19467,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
@@ -19655,7 +19655,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -19749,7 +19749,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -19843,7 +19843,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>19/11/2024</t>
+          <t>22/11/2024</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -19937,7 +19937,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -20031,7 +20031,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -20125,7 +20125,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>20/11/2024</t>
+          <t>21/11/2024</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>

</xml_diff>